<commit_message>
estado de facturacion funcionando, falta mejoras
</commit_message>
<xml_diff>
--- a/data/proveedores.xlsx
+++ b/data/proveedores.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -58,6 +58,9 @@
     <t>tami</t>
   </si>
   <si>
+    <t>Gisela porfiri proveedor</t>
+  </si>
+  <si>
     <t>20-12345678-9</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>123123124</t>
   </si>
   <si>
+    <t>123123</t>
+  </si>
+  <si>
     <t>contacto@alfa.com</t>
   </si>
   <si>
@@ -91,6 +97,9 @@
     <t>234123</t>
   </si>
   <si>
+    <t>gisela2@email.com</t>
+  </si>
+  <si>
     <t>1122334455</t>
   </si>
   <si>
@@ -103,7 +112,7 @@
     <t>312312</t>
   </si>
   <si>
-    <t>123123</t>
+    <t>12345</t>
   </si>
   <si>
     <t>Calle Falsa 123</t>
@@ -118,10 +127,13 @@
     <t>3123123s</t>
   </si>
   <si>
+    <t>del valle 462</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
     <t>Inactivo</t>
-  </si>
-  <si>
-    <t>Activo</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,19 +534,19 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -548,19 +560,19 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -574,19 +586,19 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -600,19 +612,19 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -626,19 +638,19 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -652,19 +664,45 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>